<commit_message>
Må ha samme fysisk_feltnavn
</commit_message>
<xml_diff>
--- a/data-raw/definisjoner_utledete_variabler_noric.xlsx
+++ b/data-raw/definisjoner_utledete_variabler_noric.xlsx
@@ -368,18 +368,6 @@
     <t>ki_nstemi_utredet_innen_24t()</t>
   </si>
   <si>
-    <t>indik_nstemi_angio_innen_24t_data</t>
-  </si>
-  <si>
-    <t>indik_nstemi_angio_innen_24t</t>
-  </si>
-  <si>
-    <t>indik_nstemi_angio_innen_72t_data</t>
-  </si>
-  <si>
-    <t>indik_nstemi_angio_innen_72t</t>
-  </si>
-  <si>
     <t>ki_stemi_pci_innen120min()</t>
   </si>
   <si>
@@ -488,9 +476,6 @@
     <t>SkjemastatusHovedskjema  har verdi -1 eller 0</t>
   </si>
   <si>
-    <t xml:space="preserve">Datagrunnlaget er "ja" for primærforløp hos direkte inlagte pasienter eller pasienter overført fra andre sykehus og der liggedøgn er i intervallet 0 til 60 dager.  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Antall dager mellom AnkomstPCI-sykehus og utskrivelse, denne kan også inneholde negative tider og tider over 60 dager. Brukes sammen med variabelen 'liggedogn_data'. </t>
   </si>
   <si>
@@ -659,12 +644,6 @@
     <t>ki_ak_pacemakerbehov()</t>
   </si>
   <si>
-    <t>ki_ak_pacemakerbehov_data</t>
-  </si>
-  <si>
-    <t>ki_ak_pacemakerbehov</t>
-  </si>
-  <si>
     <t>Datagrunnlaget for kvalitetsindikatoren "Pacemakerbehov etter innsetting av klaff"</t>
   </si>
   <si>
@@ -678,6 +657,27 @@
   </si>
   <si>
     <t>I datagrunnlaget og pacemaker er ikke satt inn (AvdKompPacemaker ulik  'Ja')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datagrunnlaget er "ja" for primærforløp hos direkte innlagte pasienter eller pasienter overført fra andre sykehus og der liggedøgn er i intervallet 0 til 60 dager.  </t>
+  </si>
+  <si>
+    <t>indik_nstemi_angio_innen24t_data</t>
+  </si>
+  <si>
+    <t>indik_nstemi_angio_innen24t</t>
+  </si>
+  <si>
+    <t>indik_nstemi_angio_innen72t_data</t>
+  </si>
+  <si>
+    <t>indik_nstemi_angio_innen72t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">indik_pacemakerbehov_data </t>
+  </si>
+  <si>
+    <t>indik_pacemakerbehov</t>
   </si>
 </sst>
 </file>
@@ -1032,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D109" workbookViewId="0">
-      <selection activeCell="H116" sqref="H116:H120"/>
+    <sheetView tabSelected="1" topLeftCell="E114" workbookViewId="0">
+      <selection activeCell="D118" sqref="D118:D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,25 +1057,25 @@
         <v>25</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1086,7 +1086,7 @@
         <v>26</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>1</v>
@@ -1106,7 +1106,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
@@ -1126,7 +1126,7 @@
         <v>26</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
@@ -1146,7 +1146,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>14</v>
@@ -1166,7 +1166,7 @@
         <v>26</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>0</v>
@@ -1186,7 +1186,7 @@
         <v>26</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>17</v>
@@ -1206,13 +1206,13 @@
         <v>28</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="H8" s="9">
         <v>44662</v>
@@ -1226,7 +1226,7 @@
         <v>29</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>3</v>
@@ -1246,19 +1246,19 @@
         <v>30</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="H10" s="9">
         <v>44662</v>
@@ -1272,19 +1272,19 @@
         <v>30</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H11" s="9">
         <v>44662</v>
@@ -1298,19 +1298,19 @@
         <v>30</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H12" s="9">
         <v>44662</v>
@@ -1324,19 +1324,19 @@
         <v>30</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="H13" s="9">
         <v>44662</v>
@@ -1350,19 +1350,19 @@
         <v>30</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H14" s="9">
         <v>44662</v>
@@ -1376,19 +1376,19 @@
         <v>30</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="H15" s="9">
         <v>44662</v>
@@ -1402,19 +1402,19 @@
         <v>30</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H16" s="9">
         <v>44662</v>
@@ -1428,19 +1428,19 @@
         <v>30</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="H17" s="9">
         <v>44662</v>
@@ -1454,19 +1454,19 @@
         <v>22</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>154</v>
+        <v>211</v>
       </c>
       <c r="H18" s="9">
         <v>44662</v>
@@ -1480,19 +1480,19 @@
         <v>22</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H19" s="9">
         <v>44662</v>
@@ -1506,19 +1506,19 @@
         <v>22</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H20" s="9">
         <v>44662</v>
@@ -1532,19 +1532,19 @@
         <v>22</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="H21" s="9">
         <v>44662</v>
@@ -1558,13 +1558,13 @@
         <v>22</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="H22" s="9">
         <v>44662</v>
@@ -1578,13 +1578,13 @@
         <v>38</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="H23" s="9">
         <v>44662</v>
@@ -1598,13 +1598,13 @@
         <v>40</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="H24" s="9">
         <v>44407</v>
@@ -1621,7 +1621,7 @@
         <v>41</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>43</v>
@@ -1644,7 +1644,7 @@
         <v>45</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>46</v>
@@ -1667,7 +1667,7 @@
         <v>48</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>49</v>
@@ -1690,7 +1690,7 @@
         <v>50</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>51</v>
@@ -1713,7 +1713,7 @@
         <v>50</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>52</v>
@@ -1736,7 +1736,7 @@
         <v>50</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>53</v>
@@ -1759,7 +1759,7 @@
         <v>50</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>54</v>
@@ -1782,7 +1782,7 @@
         <v>50</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>55</v>
@@ -1805,7 +1805,7 @@
         <v>50</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>56</v>
@@ -1828,7 +1828,7 @@
         <v>50</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>57</v>
@@ -1851,7 +1851,7 @@
         <v>50</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>58</v>
@@ -1874,7 +1874,7 @@
         <v>50</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>59</v>
@@ -1897,7 +1897,7 @@
         <v>50</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>60</v>
@@ -1920,7 +1920,7 @@
         <v>62</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>63</v>
@@ -1943,7 +1943,7 @@
         <v>62</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>64</v>
@@ -1966,7 +1966,7 @@
         <v>62</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>65</v>
@@ -1989,7 +1989,7 @@
         <v>62</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>66</v>
@@ -2012,7 +2012,7 @@
         <v>62</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>67</v>
@@ -2035,7 +2035,7 @@
         <v>62</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>68</v>
@@ -2058,7 +2058,7 @@
         <v>62</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>69</v>
@@ -2081,7 +2081,7 @@
         <v>62</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>70</v>
@@ -2104,7 +2104,7 @@
         <v>62</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>71</v>
@@ -2127,7 +2127,7 @@
         <v>62</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>72</v>
@@ -2150,7 +2150,7 @@
         <v>74</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>46</v>
@@ -2173,7 +2173,7 @@
         <v>75</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>76</v>
@@ -2196,7 +2196,7 @@
         <v>75</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>77</v>
@@ -2219,7 +2219,7 @@
         <v>75</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>78</v>
@@ -2242,7 +2242,7 @@
         <v>75</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>79</v>
@@ -2265,7 +2265,7 @@
         <v>75</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>80</v>
@@ -2288,7 +2288,7 @@
         <v>75</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>81</v>
@@ -2311,7 +2311,7 @@
         <v>75</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>82</v>
@@ -2334,7 +2334,7 @@
         <v>75</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>83</v>
@@ -2357,7 +2357,7 @@
         <v>75</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>84</v>
@@ -2380,7 +2380,7 @@
         <v>75</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>85</v>
@@ -2403,7 +2403,7 @@
         <v>75</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>86</v>
@@ -2426,7 +2426,7 @@
         <v>75</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>87</v>
@@ -2449,7 +2449,7 @@
         <v>75</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>88</v>
@@ -2472,7 +2472,7 @@
         <v>75</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>89</v>
@@ -2495,7 +2495,7 @@
         <v>75</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>90</v>
@@ -2518,7 +2518,7 @@
         <v>75</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>91</v>
@@ -2541,7 +2541,7 @@
         <v>75</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>92</v>
@@ -2564,7 +2564,7 @@
         <v>75</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>93</v>
@@ -2587,7 +2587,7 @@
         <v>75</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>94</v>
@@ -2610,7 +2610,7 @@
         <v>75</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>95</v>
@@ -2633,19 +2633,19 @@
         <v>98</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>99</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H69" s="9">
         <v>44662</v>
@@ -2659,19 +2659,19 @@
         <v>98</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>99</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="H70" s="9">
         <v>44662</v>
@@ -2685,19 +2685,19 @@
         <v>98</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>100</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="H71" s="9">
         <v>44662</v>
@@ -2711,19 +2711,19 @@
         <v>98</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>100</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="H72" s="9">
         <v>44662</v>
@@ -2737,19 +2737,19 @@
         <v>98</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>100</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="H73" s="9">
         <v>44662</v>
@@ -2763,19 +2763,19 @@
         <v>101</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>102</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="H74" s="9">
         <v>44662</v>
@@ -2789,19 +2789,19 @@
         <v>101</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>102</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="H75" s="9">
         <v>44662</v>
@@ -2815,19 +2815,19 @@
         <v>101</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>103</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="H76" s="9">
         <v>44662</v>
@@ -2841,19 +2841,19 @@
         <v>101</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D77" s="2" t="s">
         <v>103</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="H77" s="9">
         <v>44662</v>
@@ -2867,19 +2867,19 @@
         <v>101</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>103</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H78" s="9">
         <v>44662</v>
@@ -2893,19 +2893,19 @@
         <v>104</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D79" s="2" t="s">
         <v>105</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="H79" s="9">
         <v>44662</v>
@@ -2919,19 +2919,19 @@
         <v>104</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>105</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H80" s="9">
         <v>44662</v>
@@ -2945,19 +2945,19 @@
         <v>104</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>106</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="H81" s="9">
         <v>44662</v>
@@ -2971,19 +2971,19 @@
         <v>104</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D82" s="2" t="s">
         <v>106</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H82" s="9">
         <v>44662</v>
@@ -2997,19 +2997,19 @@
         <v>104</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D83" s="2" t="s">
         <v>106</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H83" s="9">
         <v>44662</v>
@@ -3023,19 +3023,19 @@
         <v>107</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>108</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H84" s="9">
         <v>44662</v>
@@ -3049,19 +3049,19 @@
         <v>107</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D85" s="2" t="s">
         <v>108</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H85" s="9">
         <v>44662</v>
@@ -3075,19 +3075,19 @@
         <v>107</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>109</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="H86" s="9">
         <v>44662</v>
@@ -3101,19 +3101,19 @@
         <v>107</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D87" s="2" t="s">
         <v>109</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="H87" s="9">
         <v>44662</v>
@@ -3127,19 +3127,19 @@
         <v>107</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>109</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="H88" s="9">
         <v>44662</v>
@@ -3153,19 +3153,19 @@
         <v>107</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>109</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H89" s="9">
         <v>44662</v>
@@ -3179,19 +3179,19 @@
         <v>110</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>111</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="H90" s="9">
         <v>44662</v>
@@ -3205,19 +3205,19 @@
         <v>110</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>111</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H91" s="9">
         <v>44662</v>
@@ -3231,19 +3231,19 @@
         <v>110</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>112</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="H92" s="9">
         <v>44662</v>
@@ -3257,19 +3257,19 @@
         <v>110</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>112</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="H93" s="9">
         <v>44662</v>
@@ -3283,19 +3283,19 @@
         <v>110</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>112</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="H94" s="9">
         <v>44662</v>
@@ -3309,19 +3309,19 @@
         <v>110</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>112</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H95" s="9">
         <v>44662</v>
@@ -3335,7 +3335,7 @@
         <v>31</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>32</v>
@@ -3355,19 +3355,19 @@
         <v>113</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>114</v>
+        <v>212</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="H97" s="9">
         <v>44662</v>
@@ -3381,19 +3381,19 @@
         <v>113</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>114</v>
+        <v>212</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H98" s="9">
         <v>44662</v>
@@ -3407,19 +3407,19 @@
         <v>113</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>115</v>
+        <v>213</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="H99" s="9">
         <v>44662</v>
@@ -3433,19 +3433,19 @@
         <v>113</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>115</v>
+        <v>213</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="H100" s="9">
         <v>44662</v>
@@ -3459,19 +3459,19 @@
         <v>113</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>115</v>
+        <v>213</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="H101" s="9">
         <v>44662</v>
@@ -3485,19 +3485,19 @@
         <v>113</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>115</v>
+        <v>213</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H102" s="9">
         <v>44662</v>
@@ -3508,22 +3508,22 @@
         <v>97</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>116</v>
+        <v>214</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="H103" s="9">
         <v>44662</v>
@@ -3534,22 +3534,22 @@
         <v>97</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>116</v>
+        <v>214</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H104" s="9">
         <v>44662</v>
@@ -3560,22 +3560,22 @@
         <v>97</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>117</v>
+        <v>215</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="H105" s="9">
         <v>44662</v>
@@ -3586,22 +3586,22 @@
         <v>97</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>117</v>
+        <v>215</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="H106" s="9">
         <v>44662</v>
@@ -3612,22 +3612,22 @@
         <v>97</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>117</v>
+        <v>215</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="H107" s="9">
         <v>44662</v>
@@ -3638,22 +3638,22 @@
         <v>97</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>117</v>
+        <v>215</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H108" s="9">
         <v>44662</v>
@@ -3667,7 +3667,7 @@
         <v>34</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>35</v>
@@ -3684,22 +3684,22 @@
         <v>97</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="H110" s="9">
         <v>44662</v>
@@ -3710,22 +3710,22 @@
         <v>97</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C111" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H111" s="9">
         <v>44662</v>
@@ -3736,22 +3736,22 @@
         <v>97</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H112" s="9">
         <v>44662</v>
@@ -3762,22 +3762,22 @@
         <v>97</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="H113" s="9">
         <v>44662</v>
@@ -3788,22 +3788,22 @@
         <v>97</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="H114" s="9">
         <v>44662</v>
@@ -3814,22 +3814,22 @@
         <v>97</v>
       </c>
       <c r="B115" s="7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H115" s="9">
         <v>44662</v>
@@ -3840,22 +3840,22 @@
         <v>97</v>
       </c>
       <c r="B116" s="7" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H116" s="9">
         <v>44662</v>
@@ -3866,22 +3866,22 @@
         <v>97</v>
       </c>
       <c r="B117" s="7" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H117" s="9">
         <v>44662</v>
@@ -3892,22 +3892,22 @@
         <v>97</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="H118" s="9">
         <v>44662</v>
@@ -3918,22 +3918,22 @@
         <v>97</v>
       </c>
       <c r="B119" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="C119" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G119" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="C119" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="D119" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="E119" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G119" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="H119" s="9">
         <v>44662</v>
@@ -3944,22 +3944,22 @@
         <v>97</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H120" s="9">
         <v>44662</v>

</xml_diff>